<commit_message>
fix aligment in gt4 sheet
</commit_message>
<xml_diff>
--- a/templates/manager_signin.xlsx
+++ b/templates/manager_signin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E5EFF8-4EAD-554F-8827-30C13B147DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675583B9-4571-6240-8862-36733870CAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{542D648B-9180-43EF-9053-182057C63D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="GTWCA" sheetId="1" r:id="rId1"/>
@@ -1102,9 +1102,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1223,60 +1220,63 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="37" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1287,6 +1287,148 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{561A9865-CE34-4D81-A124-2143BF703225}"/>
   </cellStyles>
   <dxfs count="48">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color auto="1"/>
+        <name val="Calibri (Body)"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1312,143 +1454,6 @@
         </left>
         <right style="thin">
           <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="22"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
@@ -1499,95 +1504,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color auto="1"/>
-        <name val="Calibri (Body)"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
@@ -1698,6 +1614,36 @@
         <bottom style="thick">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1889,6 +1835,33 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2073,6 +2046,33 @@
         <bottom style="thick">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2154,18 +2154,60 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thick">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="24"/>
+        <sz val="22"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2178,19 +2220,20 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="24"/>
+        <sz val="12"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2202,36 +2245,6 @@
           <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thick">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thick">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -2287,46 +2300,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="26"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -2433,6 +2406,33 @@
         <bottom style="thick">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2738,28 +2738,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A8ED4E7-BF26-42C3-BDB6-D75B0242E935}" name="Table22" displayName="Table22" ref="A7:D23" totalsRowShown="0" headerRowDxfId="3" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A8ED4E7-BF26-42C3-BDB6-D75B0242E935}" name="Table22" displayName="Table22" ref="A7:D23" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D19">
     <sortCondition ref="A7:A19"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{46535ACF-119B-47E2-B654-91600EA2F824}" name="Team " dataDxfId="42" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{7167445C-3407-834C-B9FA-DB045AAEB2B5}" name="Car #" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{F83754C0-485E-4A3F-9902-121B9D0452B7}" name="Print Name" dataDxfId="40" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{B3757E69-E5A4-4C14-936E-7FBD8332261E}" name="Signature" dataDxfId="39" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{46535ACF-119B-47E2-B654-91600EA2F824}" name="Team " dataDxfId="41" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{7167445C-3407-834C-B9FA-DB045AAEB2B5}" name="Car #" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{F83754C0-485E-4A3F-9902-121B9D0452B7}" name="Print Name" dataDxfId="39" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{B3757E69-E5A4-4C14-936E-7FBD8332261E}" name="Signature" dataDxfId="38" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D38" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{56F25BC1-6701-4669-AC0F-E1673995674A}" name="Table2267" displayName="Table2267" ref="A7:D38" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D29">
     <sortCondition ref="A7:A29"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="35" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{C0375D1B-A6A9-4878-94F1-144B367DBFAE}" name="Team " dataDxfId="1" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{72AB2F61-1891-C246-9F82-F99E634034BF}" name="Car #" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{731AF936-9BBC-4114-AF94-6737C2C799AD}" name="Print Name" dataDxfId="33" dataCellStyle="Neutral"/>
     <tableColumn id="5" xr3:uid="{4AAAC599-A742-4343-8BE4-F0207EAEB236}" name="Signature" dataDxfId="32" dataCellStyle="Neutral"/>
   </tableColumns>
@@ -2768,61 +2768,61 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EEF14E4E-087A-46C7-831D-A668229E00D6}" name="Table226" displayName="Table226" ref="A7:D28" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D28">
     <sortCondition ref="A7:A28"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="27" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{35983ADC-4C21-324B-8F2F-BF0F688AF0E7}" name="Car #" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Team Manager - Print Name" dataDxfId="25" dataCellStyle="Neutral"/>
-    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Signature" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{9FCCBAF6-EB7D-44F1-ADEC-A2DF74A549AE}" name="Team " dataDxfId="26" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{35983ADC-4C21-324B-8F2F-BF0F688AF0E7}" name="Car #" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{5972D2A1-6086-4595-9053-F6AB4ABD85A7}" name="Team Manager - Print Name" dataDxfId="24" dataCellStyle="Neutral"/>
+    <tableColumn id="7" xr3:uid="{7B3018A6-2A70-4C3E-BE5C-CCFFCABD4796}" name="Signature" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7C975FDB-E1BE-412D-9026-C8BCE6F82D94}" name="Table2268" displayName="Table2268" ref="A7:D26" totalsRowShown="0" headerRowDxfId="2" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{7C975FDB-E1BE-412D-9026-C8BCE6F82D94}" name="Table2268" displayName="Table2268" ref="A7:D26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D20">
     <sortCondition ref="A8:A20"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="3" xr3:uid="{9A87D9F1-DEF9-4884-AF55-85CDAB8CC5A8}" name="Team " dataDxfId="19" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{A77D3C38-62D3-EB45-842F-39E925EA4278}" name="Car #" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{FB87E8C6-0099-4FD3-9EE4-DC66B1A1E154}" name="Print Name" dataDxfId="17" dataCellStyle="Neutral"/>
-    <tableColumn id="8" xr3:uid="{D99F6B7B-0B67-4A5D-8961-35323F63E14D}" name="Signature" dataDxfId="16" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{9A87D9F1-DEF9-4884-AF55-85CDAB8CC5A8}" name="Team " dataDxfId="17" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{A77D3C38-62D3-EB45-842F-39E925EA4278}" name="Car #" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{FB87E8C6-0099-4FD3-9EE4-DC66B1A1E154}" name="Print Name" dataDxfId="15" dataCellStyle="Neutral"/>
+    <tableColumn id="8" xr3:uid="{D99F6B7B-0B67-4A5D-8961-35323F63E14D}" name="Signature" dataDxfId="14" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34633D1F-F7E7-A54F-B80A-2DBC56A5E286}" name="Table4" displayName="Table4" ref="A7:D24" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="15" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34633D1F-F7E7-A54F-B80A-2DBC56A5E286}" name="Table4" displayName="Table4" ref="A7:D24" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A7:D24" xr:uid="{34633D1F-F7E7-A54F-B80A-2DBC56A5E286}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:D24">
     <sortCondition ref="A7:A24"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{5F92970B-06CD-C047-B9E2-6AB880B6FB5E}" name="Team " dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{54681146-35F4-D54D-9BC0-D686C4A484BC}" name="Car #" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{7B238E6B-1F96-FC45-8097-E871888A60A5}" name="Print Name" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{9A683F97-A1BA-904F-8CF4-974B16662D90}" name="Signature" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{5F92970B-06CD-C047-B9E2-6AB880B6FB5E}" name="Team " dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{54681146-35F4-D54D-9BC0-D686C4A484BC}" name="Car #" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{7B238E6B-1F96-FC45-8097-E871888A60A5}" name="Print Name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{9A683F97-A1BA-904F-8CF4-974B16662D90}" name="Signature" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}" name="Table2" displayName="Table2" ref="A7:C72" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}" name="Table2" displayName="Table2" ref="A7:C72" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A7:C72" xr:uid="{5C8910A9-D883-CB47-ADF7-2489AEA18D68}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:C72">
     <sortCondition ref="A7:A72"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{AD000ADB-6327-CD45-BE99-F1047C0BF216}" name="Team " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AD000ADB-6327-CD45-BE99-F1047C0BF216}" name="Team " dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{CDB7A7EE-F7C4-DE41-B5A3-3A45AA9CEAAC}" name="Print Name"/>
-    <tableColumn id="4" xr3:uid="{66076889-B43A-3746-B4F7-4CFF3E5423AA}" name="Signature" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{66076889-B43A-3746-B4F7-4CFF3E5423AA}" name="Signature" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3144,126 +3144,126 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174"/>
-      <c r="B2" s="176" t="s">
+      <c r="A2" s="184"/>
+      <c r="B2" s="185" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="174"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
+      <c r="A3" s="184"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="186"/>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="181" t="s">
+      <c r="A7" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="181" t="s">
+      <c r="B7" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="181" t="s">
+      <c r="C7" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="181" t="s">
+      <c r="D7" s="175" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="135"/>
-      <c r="B8" s="136"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="137"/>
-      <c r="B9" s="138"/>
+      <c r="A9" s="136"/>
+      <c r="B9" s="137"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="137"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="139"/>
-      <c r="B11" s="136"/>
+      <c r="A11" s="138"/>
+      <c r="B11" s="135"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="137"/>
-      <c r="B12" s="138"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="137"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="140"/>
-      <c r="B13" s="136"/>
+      <c r="A13" s="139"/>
+      <c r="B13" s="135"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="137"/>
-      <c r="B14" s="136"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="139"/>
-      <c r="B15" s="138"/>
+      <c r="A15" s="138"/>
+      <c r="B15" s="137"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="137"/>
-      <c r="B16" s="138"/>
+      <c r="A16" s="136"/>
+      <c r="B16" s="137"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="141"/>
-      <c r="B17" s="142"/>
+      <c r="A17" s="140"/>
+      <c r="B17" s="141"/>
       <c r="C17" s="64"/>
       <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="143"/>
-      <c r="B18" s="138"/>
+      <c r="A18" s="142"/>
+      <c r="B18" s="137"/>
       <c r="C18" s="63"/>
       <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" s="18" customFormat="1" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="144"/>
-      <c r="B19" s="138"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="137"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
     <row r="20" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="137"/>
-      <c r="B20" s="145"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="144"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="137"/>
-      <c r="B21" s="145"/>
+      <c r="A21" s="136"/>
+      <c r="B21" s="144"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="137"/>
-      <c r="B22" s="145"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="144"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="146"/>
-      <c r="B23" s="147"/>
+      <c r="A23" s="145"/>
+      <c r="B23" s="146"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
     </row>
@@ -3289,8 +3289,8 @@
   </sheetPr>
   <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView view="pageLayout" topLeftCell="A31" zoomScale="90" zoomScaleNormal="115" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3302,42 +3302,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174"/>
-      <c r="B2" s="178" t="s">
+      <c r="A2" s="184"/>
+      <c r="B2" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="174"/>
-      <c r="B3" s="178"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="178"/>
+      <c r="A3" s="184"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="174"/>
-      <c r="B4" s="178"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
+      <c r="A4" s="184"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="174"/>
-      <c r="B5" s="178"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
+      <c r="A5" s="184"/>
+      <c r="B5" s="187"/>
+      <c r="C5" s="187"/>
+      <c r="D5" s="187"/>
     </row>
     <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="180" t="s">
+      <c r="A7" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="180" t="s">
+      <c r="B7" s="174" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="180" t="s">
+      <c r="C7" s="174" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="180" t="s">
+      <c r="D7" s="174" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3473,57 +3473,57 @@
       <c r="C29" s="8"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="132"/>
-      <c r="B30" s="133"/>
+      <c r="B30" s="191"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="132"/>
-      <c r="B31" s="133"/>
+      <c r="B31" s="191"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="132"/>
-      <c r="B32" s="133"/>
+      <c r="B32" s="191"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="132"/>
-      <c r="B33" s="133"/>
+      <c r="B33" s="191"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="132"/>
-      <c r="B34" s="133"/>
+      <c r="B34" s="191"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="132"/>
-      <c r="B35" s="133"/>
+      <c r="B35" s="191"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="132"/>
-      <c r="B36" s="133"/>
+      <c r="B36" s="191"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="132"/>
-      <c r="B37" s="133"/>
+      <c r="B37" s="191"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="134"/>
-      <c r="B38" s="133"/>
+    <row r="38" spans="1:4" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="133"/>
+      <c r="B38" s="191"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
@@ -3549,8 +3549,8 @@
   </sheetPr>
   <dimension ref="A2:D30"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="80" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3562,42 +3562,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174"/>
-      <c r="B2" s="178" t="s">
+      <c r="A2" s="184"/>
+      <c r="B2" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="174"/>
-      <c r="B3" s="178"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="178"/>
+      <c r="A3" s="184"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
     </row>
     <row r="4" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="174"/>
-      <c r="B4" s="178"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
+      <c r="A4" s="184"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
     </row>
     <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="174"/>
-      <c r="B5" s="178"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
+      <c r="A5" s="184"/>
+      <c r="B5" s="187"/>
+      <c r="C5" s="187"/>
+      <c r="D5" s="187"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179" t="s">
+      <c r="A7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="179" t="s">
+      <c r="B7" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="179" t="s">
+      <c r="D7" s="173" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3780,51 +3780,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="A1" s="174"/>
-      <c r="B1" s="178" t="s">
+      <c r="A1" s="184"/>
+      <c r="B1" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="A2" s="174"/>
-      <c r="B2" s="178"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
+      <c r="A2" s="184"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
     </row>
     <row r="3" spans="1:88" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="174"/>
-      <c r="B3" s="178"/>
-      <c r="C3" s="178"/>
-      <c r="D3" s="178"/>
+      <c r="A3" s="184"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
     </row>
     <row r="4" spans="1:88" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="174"/>
-      <c r="B4" s="178"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
+      <c r="A4" s="184"/>
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
     </row>
     <row r="5" spans="1:88" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="174"/>
+      <c r="A5" s="184"/>
       <c r="C5" s="120"/>
       <c r="D5" s="120"/>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="F6" s="174"/>
-      <c r="G6" s="174"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="184"/>
     </row>
     <row r="7" spans="1:88" s="17" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="182" t="s">
+      <c r="A7" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="183" t="s">
+      <c r="C7" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="182" t="s">
+      <c r="D7" s="176" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="36"/>
@@ -4003,7 +4003,7 @@
       <c r="CJ8" s="37"/>
     </row>
     <row r="9" spans="1:88" s="17" customFormat="1" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="150"/>
+      <c r="A9" s="149"/>
       <c r="B9" s="89"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
@@ -4093,7 +4093,7 @@
       <c r="CJ9" s="37"/>
     </row>
     <row r="10" spans="1:88" s="17" customFormat="1" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="150"/>
+      <c r="A10" s="149"/>
       <c r="B10" s="89"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -4633,7 +4633,7 @@
       <c r="CJ15" s="37"/>
     </row>
     <row r="16" spans="1:88" s="17" customFormat="1" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="150"/>
+      <c r="A16" s="149"/>
       <c r="B16" s="112"/>
       <c r="C16" s="8"/>
       <c r="D16" s="42"/>
@@ -5083,40 +5083,40 @@
       <c r="CJ20" s="37"/>
     </row>
     <row r="21" spans="1:88" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="150"/>
+      <c r="A21" s="149"/>
       <c r="B21" s="89"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:88" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="150"/>
+      <c r="A22" s="149"/>
       <c r="B22" s="89"/>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:88" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="150"/>
+      <c r="A23" s="149"/>
       <c r="B23" s="89"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:88" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="150"/>
+      <c r="A24" s="149"/>
       <c r="B24" s="89"/>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:88" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="150"/>
+      <c r="A25" s="149"/>
       <c r="B25" s="89"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:88" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="151"/>
-      <c r="B26" s="148"/>
+      <c r="A26" s="150"/>
+      <c r="B26" s="147"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="149"/>
+      <c r="D26" s="148"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5154,12 +5154,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="184"/>
-      <c r="B1" s="185" t="s">
+      <c r="A1" s="188"/>
+      <c r="B1" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
@@ -5167,10 +5167,10 @@
       <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="184"/>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
+      <c r="A2" s="188"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
@@ -5178,10 +5178,10 @@
       <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="184"/>
-      <c r="B3" s="185"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
+      <c r="A3" s="188"/>
+      <c r="B3" s="189"/>
+      <c r="C3" s="189"/>
+      <c r="D3" s="189"/>
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -5189,10 +5189,10 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="184"/>
-      <c r="B4" s="185"/>
-      <c r="C4" s="185"/>
-      <c r="D4" s="185"/>
+      <c r="A4" s="188"/>
+      <c r="B4" s="189"/>
+      <c r="C4" s="189"/>
+      <c r="D4" s="189"/>
       <c r="E4" s="24"/>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
@@ -5200,10 +5200,10 @@
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="184"/>
-      <c r="B5" s="185"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
+      <c r="A5" s="188"/>
+      <c r="B5" s="189"/>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
@@ -5222,16 +5222,16 @@
       <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="188" t="s">
+      <c r="A7" s="180" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="189" t="s">
+      <c r="B7" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="190" t="s">
+      <c r="C7" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="191" t="s">
+      <c r="D7" s="183" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="24"/>
@@ -5461,7 +5461,7 @@
   </sheetPr>
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -5473,11 +5473,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="92" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
     </row>
     <row r="2" spans="1:3" ht="5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="58"/>
@@ -5493,63 +5493,63 @@
     </row>
     <row r="6" spans="1:3" ht="8" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:3" ht="26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="186" t="s">
+      <c r="A7" s="178" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="183" t="s">
+      <c r="B7" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="187" t="s">
+      <c r="C7" s="179" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="152"/>
+      <c r="A8" s="151"/>
       <c r="B8" s="53"/>
       <c r="C8" s="50"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="153"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="53"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="154"/>
+      <c r="A10" s="153"/>
       <c r="B10" s="53"/>
       <c r="C10" s="50"/>
     </row>
     <row r="11" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="155"/>
+      <c r="A11" s="154"/>
       <c r="B11" s="53"/>
       <c r="C11" s="50"/>
     </row>
     <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="156"/>
+      <c r="A12" s="155"/>
       <c r="B12" s="53"/>
       <c r="C12" s="50"/>
     </row>
     <row r="13" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="152"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="53"/>
       <c r="C13" s="50"/>
     </row>
     <row r="14" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
+      <c r="A14" s="156"/>
       <c r="B14" s="53"/>
       <c r="C14" s="50"/>
     </row>
     <row r="15" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="158"/>
+      <c r="A15" s="157"/>
       <c r="B15" s="53"/>
       <c r="C15" s="50"/>
     </row>
     <row r="16" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="152"/>
+      <c r="A16" s="151"/>
       <c r="B16" s="53"/>
       <c r="C16" s="52"/>
     </row>
     <row r="17" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="159"/>
+      <c r="A17" s="158"/>
       <c r="B17" s="55"/>
       <c r="C17" s="50"/>
     </row>
@@ -5559,7 +5559,7 @@
       <c r="C18" s="50"/>
     </row>
     <row r="19" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="154"/>
+      <c r="A19" s="153"/>
       <c r="B19" s="55"/>
       <c r="C19" s="50"/>
     </row>
@@ -5569,32 +5569,32 @@
       <c r="C20" s="50"/>
     </row>
     <row r="21" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="157"/>
+      <c r="A21" s="156"/>
       <c r="B21" s="55"/>
       <c r="C21" s="50"/>
     </row>
     <row r="22" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="154"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="55"/>
       <c r="C22" s="50"/>
     </row>
     <row r="23" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="160"/>
+      <c r="A23" s="159"/>
       <c r="B23" s="55"/>
       <c r="C23" s="50"/>
     </row>
     <row r="24" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="154"/>
+      <c r="A24" s="153"/>
       <c r="B24" s="55"/>
       <c r="C24" s="50"/>
     </row>
     <row r="25" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="154"/>
+      <c r="A25" s="153"/>
       <c r="B25" s="55"/>
       <c r="C25" s="50"/>
     </row>
     <row r="26" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="157"/>
+      <c r="A26" s="156"/>
       <c r="B26" s="55"/>
       <c r="C26" s="50"/>
     </row>
@@ -5609,102 +5609,102 @@
       <c r="C28" s="50"/>
     </row>
     <row r="29" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="161"/>
+      <c r="A29" s="160"/>
       <c r="B29" s="55"/>
       <c r="C29" s="50"/>
     </row>
     <row r="30" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="157"/>
+      <c r="A30" s="156"/>
       <c r="B30" s="55"/>
       <c r="C30" s="50"/>
     </row>
     <row r="31" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="162"/>
+      <c r="A31" s="161"/>
       <c r="B31" s="55"/>
       <c r="C31" s="50"/>
     </row>
     <row r="32" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="160"/>
+      <c r="A32" s="159"/>
       <c r="B32" s="55"/>
       <c r="C32" s="50"/>
     </row>
     <row r="33" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="152"/>
+      <c r="A33" s="151"/>
       <c r="B33" s="55"/>
       <c r="C33" s="50"/>
     </row>
     <row r="34" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="154"/>
+      <c r="A34" s="153"/>
       <c r="B34" s="55"/>
       <c r="C34" s="50"/>
     </row>
     <row r="35" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="163"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="55"/>
       <c r="C35" s="50"/>
     </row>
     <row r="36" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="161"/>
+      <c r="A36" s="160"/>
       <c r="B36" s="55"/>
       <c r="C36" s="50"/>
     </row>
     <row r="37" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="157"/>
+      <c r="A37" s="156"/>
       <c r="B37" s="55"/>
       <c r="C37" s="50"/>
     </row>
     <row r="38" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="164"/>
+      <c r="A38" s="163"/>
       <c r="B38" s="55"/>
       <c r="C38" s="50"/>
     </row>
     <row r="39" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="154"/>
+      <c r="A39" s="153"/>
       <c r="B39" s="55"/>
       <c r="C39" s="50"/>
     </row>
     <row r="40" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="152"/>
+      <c r="A40" s="151"/>
       <c r="B40" s="57"/>
       <c r="C40" s="50"/>
     </row>
     <row r="41" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="153"/>
+      <c r="A41" s="152"/>
       <c r="B41" s="55"/>
       <c r="C41" s="50"/>
     </row>
     <row r="42" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="153"/>
+      <c r="A42" s="152"/>
       <c r="B42" s="55"/>
       <c r="C42" s="50"/>
     </row>
     <row r="43" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="165"/>
+      <c r="A43" s="164"/>
       <c r="B43" s="55"/>
       <c r="C43" s="50"/>
     </row>
     <row r="44" spans="1:3" s="111" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="160"/>
+      <c r="A44" s="159"/>
       <c r="B44" s="109"/>
       <c r="C44" s="110"/>
     </row>
     <row r="45" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="153"/>
+      <c r="A45" s="152"/>
       <c r="B45" s="55"/>
       <c r="C45" s="50"/>
     </row>
     <row r="46" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="153"/>
+      <c r="A46" s="152"/>
       <c r="B46" s="55"/>
       <c r="C46" s="50"/>
     </row>
     <row r="47" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="153"/>
+      <c r="A47" s="152"/>
       <c r="B47" s="55"/>
       <c r="C47" s="50"/>
     </row>
     <row r="48" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="157"/>
+      <c r="A48" s="156"/>
       <c r="B48" s="55"/>
       <c r="C48" s="50"/>
     </row>
@@ -5714,37 +5714,37 @@
       <c r="C49" s="50"/>
     </row>
     <row r="50" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="166"/>
+      <c r="A50" s="165"/>
       <c r="B50" s="55"/>
       <c r="C50" s="50"/>
     </row>
     <row r="51" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="154"/>
+      <c r="A51" s="153"/>
       <c r="B51" s="26"/>
       <c r="C51" s="51"/>
     </row>
     <row r="52" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="167"/>
+      <c r="A52" s="166"/>
       <c r="B52" s="55"/>
       <c r="C52" s="50"/>
     </row>
     <row r="53" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="168"/>
+      <c r="A53" s="167"/>
       <c r="B53" s="55"/>
       <c r="C53" s="50"/>
     </row>
     <row r="54" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="154"/>
+      <c r="A54" s="153"/>
       <c r="B54" s="56"/>
       <c r="C54" s="50"/>
     </row>
     <row r="55" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="153"/>
+      <c r="A55" s="152"/>
       <c r="B55" s="55"/>
       <c r="C55" s="50"/>
     </row>
     <row r="56" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="169"/>
+      <c r="A56" s="168"/>
       <c r="B56" s="55"/>
       <c r="C56" s="50"/>
     </row>
@@ -5754,7 +5754,7 @@
       <c r="C57" s="50"/>
     </row>
     <row r="58" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="154"/>
+      <c r="A58" s="153"/>
       <c r="B58" s="55"/>
       <c r="C58" s="50"/>
     </row>
@@ -5764,67 +5764,67 @@
       <c r="C59" s="50"/>
     </row>
     <row r="60" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="167"/>
+      <c r="A60" s="166"/>
       <c r="B60" s="27"/>
       <c r="C60" s="50"/>
     </row>
     <row r="61" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="155"/>
+      <c r="A61" s="154"/>
       <c r="B61" s="53"/>
       <c r="C61" s="50"/>
     </row>
     <row r="62" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="170"/>
+      <c r="A62" s="169"/>
       <c r="B62" s="53"/>
       <c r="C62" s="50"/>
     </row>
     <row r="63" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="170"/>
+      <c r="A63" s="169"/>
       <c r="B63" s="53"/>
       <c r="C63" s="50"/>
     </row>
     <row r="64" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="171"/>
+      <c r="A64" s="170"/>
       <c r="B64" s="53"/>
       <c r="C64" s="50"/>
     </row>
     <row r="65" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="158"/>
+      <c r="A65" s="157"/>
       <c r="B65" s="53"/>
       <c r="C65" s="52"/>
     </row>
     <row r="66" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="167"/>
+      <c r="A66" s="166"/>
       <c r="B66" s="53"/>
       <c r="C66" s="50"/>
     </row>
     <row r="67" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="167"/>
+      <c r="A67" s="166"/>
       <c r="B67" s="53"/>
       <c r="C67" s="50"/>
     </row>
     <row r="68" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="161"/>
+      <c r="A68" s="160"/>
       <c r="B68" s="53"/>
       <c r="C68" s="50"/>
     </row>
     <row r="69" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="167"/>
+      <c r="A69" s="166"/>
       <c r="B69" s="53"/>
       <c r="C69" s="50"/>
     </row>
     <row r="70" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="161"/>
+      <c r="A70" s="160"/>
       <c r="B70" s="53"/>
       <c r="C70" s="50"/>
     </row>
     <row r="71" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="172"/>
+      <c r="A71" s="171"/>
       <c r="B71" s="53"/>
       <c r="C71" s="50"/>
     </row>
     <row r="72" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="173"/>
+      <c r="A72" s="172"/>
       <c r="C72" s="50"/>
     </row>
   </sheetData>
@@ -5840,14 +5840,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6088,21 +6086,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c298f69c-7e32-4d69-8a4f-44b776bc75e5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="27d18e64-52d1-4030-b5cf-9c691bb829da" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
-    <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6127,9 +6124,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18B17227-D4F1-4BA2-A533-34BDC1F9C7F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B37A3888-C326-48DF-AE4A-829BED1A658A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c298f69c-7e32-4d69-8a4f-44b776bc75e5"/>
+    <ds:schemaRef ds:uri="27d18e64-52d1-4030-b5cf-9c691bb829da"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>